<commit_message>
updated names and roles
</commit_message>
<xml_diff>
--- a/Misc/Names and Roles.xlsx
+++ b/Misc/Names and Roles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ShiMapleLeaf\Documents\Parallel Heroes\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E040565-7895-474B-A73C-D2B67A71CC6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDCF46F-4EA5-4982-8F4B-495228359932}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{EF0C7BE9-5DEA-4A5F-B898-9F15494C8668}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EF0C7BE9-5DEA-4A5F-B898-9F15494C8668}"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -3887,7 +3887,7 @@
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T39" sqref="T39"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -3964,29 +3964,29 @@
         <v>93</v>
       </c>
       <c r="G2" s="2">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="H2" s="2">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="I2" s="2">
+        <v>65</v>
+      </c>
+      <c r="J2" s="2">
         <v>55</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="2">
         <v>45</v>
       </c>
-      <c r="K2" s="2">
-        <v>35</v>
-      </c>
       <c r="L2" s="2">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="M2" s="2">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="N2" s="2">
         <f>SUM(G2:M2)</f>
-        <v>315</v>
+        <v>385</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -4075,29 +4075,29 @@
         <v>132</v>
       </c>
       <c r="G7" s="2">
+        <v>65</v>
+      </c>
+      <c r="H7" s="2">
         <v>55</v>
       </c>
-      <c r="H7" s="2">
-        <v>45</v>
-      </c>
       <c r="I7" s="2">
+        <v>65</v>
+      </c>
+      <c r="J7" s="2">
+        <v>50</v>
+      </c>
+      <c r="K7" s="2">
         <v>55</v>
       </c>
-      <c r="J7" s="2">
+      <c r="L7" s="2">
         <v>40</v>
       </c>
-      <c r="K7" s="2">
-        <v>45</v>
-      </c>
-      <c r="L7" s="2">
-        <v>30</v>
-      </c>
       <c r="M7" s="2">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="N7" s="2">
         <f t="shared" si="0"/>
-        <v>315</v>
+        <v>385</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -4276,29 +4276,29 @@
         <v>95</v>
       </c>
       <c r="G17" s="2">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="H17" s="2">
+        <v>70</v>
+      </c>
+      <c r="I17" s="2">
         <v>60</v>
       </c>
-      <c r="I17" s="2">
-        <v>50</v>
-      </c>
       <c r="J17" s="2">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="K17" s="2">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="L17" s="2">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="M17" s="2">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="N17" s="2">
         <f t="shared" si="0"/>
-        <v>315</v>
+        <v>385</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
@@ -4333,29 +4333,29 @@
         <v>131</v>
       </c>
       <c r="G19" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="H19" s="2">
+        <v>70</v>
+      </c>
+      <c r="I19" s="2">
+        <v>60</v>
+      </c>
+      <c r="J19" s="2">
         <v>50</v>
       </c>
-      <c r="I19" s="2">
-        <v>50</v>
-      </c>
-      <c r="J19" s="2">
-        <v>40</v>
-      </c>
       <c r="K19" s="2">
+        <v>55</v>
+      </c>
+      <c r="L19" s="2">
+        <v>60</v>
+      </c>
+      <c r="M19" s="2">
         <v>45</v>
-      </c>
-      <c r="L19" s="2">
-        <v>50</v>
-      </c>
-      <c r="M19" s="2">
-        <v>40</v>
       </c>
       <c r="N19" s="2">
         <f t="shared" si="0"/>
-        <v>315</v>
+        <v>390</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fricking names and roles file uhg
</commit_message>
<xml_diff>
--- a/Misc/Names and Roles.xlsx
+++ b/Misc/Names and Roles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ShiMapleLeaf\Documents\Parallel Heroes\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B0F950-0B26-43DD-BB9E-291B0C89A91D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92440C2B-3FAF-4217-8FA2-89271B4DDA5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{EF0C7BE9-5DEA-4A5F-B898-9F15494C8668}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EF0C7BE9-5DEA-4A5F-B898-9F15494C8668}"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="137">
   <si>
     <t>Clint</t>
   </si>
@@ -440,6 +440,9 @@
   </si>
   <si>
     <t>Cash</t>
+  </si>
+  <si>
+    <t>Lute</t>
   </si>
 </sst>
 </file>
@@ -559,7 +562,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3893,7 +3896,7 @@
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S28" sqref="S28"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -4261,11 +4264,32 @@
         <v>24</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>104</v>
+        <v>136</v>
+      </c>
+      <c r="G16" s="2">
+        <v>50</v>
+      </c>
+      <c r="H16" s="2">
+        <v>65</v>
+      </c>
+      <c r="I16" s="2">
+        <v>50</v>
+      </c>
+      <c r="J16" s="2">
+        <v>50</v>
+      </c>
+      <c r="K16" s="2">
+        <v>70</v>
+      </c>
+      <c r="L16" s="2">
+        <v>40</v>
+      </c>
+      <c r="M16" s="2">
+        <v>60</v>
       </c>
       <c r="N16" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>385</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
names and roles update
</commit_message>
<xml_diff>
--- a/Misc/Names and Roles.xlsx
+++ b/Misc/Names and Roles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ShiMapleLeaf\Documents\Parallel Heroes\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92440C2B-3FAF-4217-8FA2-89271B4DDA5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3E50BA-1EF3-4EDD-AFE0-408EF1907852}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EF0C7BE9-5DEA-4A5F-B898-9F15494C8668}"/>
   </bookViews>
@@ -662,7 +662,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp38.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp39.xml><?xml version="1.0" encoding="utf-8"?>
@@ -674,7 +674,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp40.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp41.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3895,8 +3895,8 @@
   <sheetPr codeName="Blad1"/>
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -4786,9 +4786,30 @@
       <c r="D39" s="2" t="s">
         <v>116</v>
       </c>
+      <c r="G39" s="2">
+        <v>45</v>
+      </c>
+      <c r="H39" s="2">
+        <v>60</v>
+      </c>
+      <c r="I39" s="2">
+        <v>75</v>
+      </c>
+      <c r="J39" s="2">
+        <v>50</v>
+      </c>
+      <c r="K39" s="2">
+        <v>45</v>
+      </c>
+      <c r="L39" s="2">
+        <v>60</v>
+      </c>
+      <c r="M39" s="2">
+        <v>50</v>
+      </c>
       <c r="N39" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>385</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
@@ -4822,9 +4843,30 @@
       <c r="D41" s="2" t="s">
         <v>107</v>
       </c>
+      <c r="G41" s="2">
+        <v>70</v>
+      </c>
+      <c r="H41" s="2">
+        <v>50</v>
+      </c>
+      <c r="I41" s="2">
+        <v>60</v>
+      </c>
+      <c r="J41" s="2">
+        <v>45</v>
+      </c>
+      <c r="K41" s="2">
+        <v>55</v>
+      </c>
+      <c r="L41" s="2">
+        <v>40</v>
+      </c>
+      <c r="M41" s="2">
+        <v>70</v>
+      </c>
       <c r="N41" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>390</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added Slim the Knight
</commit_message>
<xml_diff>
--- a/Misc/Names and Roles.xlsx
+++ b/Misc/Names and Roles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ShiMapleLeaf\Documents\Parallel Heroes\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3E50BA-1EF3-4EDD-AFE0-408EF1907852}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C005A01-D9F5-4734-B706-1E28D66ACC91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EF0C7BE9-5DEA-4A5F-B898-9F15494C8668}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{EF0C7BE9-5DEA-4A5F-B898-9F15494C8668}"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -670,7 +670,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp40.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3895,8 +3895,8 @@
   <sheetPr codeName="Blad1"/>
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -4047,9 +4047,30 @@
       <c r="D5" s="2" t="s">
         <v>96</v>
       </c>
+      <c r="G5" s="2">
+        <v>85</v>
+      </c>
+      <c r="H5" s="2">
+        <v>40</v>
+      </c>
+      <c r="I5" s="2">
+        <v>70</v>
+      </c>
+      <c r="J5" s="2">
+        <v>85</v>
+      </c>
+      <c r="K5" s="2">
+        <v>15</v>
+      </c>
+      <c r="L5" s="2">
+        <v>55</v>
+      </c>
+      <c r="M5" s="2">
+        <v>35</v>
+      </c>
       <c r="N5" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>385</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added Olaf the Viking
</commit_message>
<xml_diff>
--- a/Misc/Names and Roles.xlsx
+++ b/Misc/Names and Roles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ShiMapleLeaf\Documents\Parallel Heroes\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C005A01-D9F5-4734-B706-1E28D66ACC91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F86CE90-9FE7-4F47-A4DB-3F60A62DD1F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{EF0C7BE9-5DEA-4A5F-B898-9F15494C8668}"/>
   </bookViews>
@@ -650,7 +650,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp35.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp36.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3896,7 +3896,7 @@
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -4753,9 +4753,30 @@
       <c r="D36" s="2" t="s">
         <v>114</v>
       </c>
+      <c r="G36" s="2">
+        <v>55</v>
+      </c>
+      <c r="H36" s="2">
+        <v>55</v>
+      </c>
+      <c r="I36" s="2">
+        <v>55</v>
+      </c>
+      <c r="J36" s="2">
+        <v>55</v>
+      </c>
+      <c r="K36" s="2">
+        <v>55</v>
+      </c>
+      <c r="L36" s="2">
+        <v>55</v>
+      </c>
+      <c r="M36" s="2">
+        <v>55</v>
+      </c>
       <c r="N36" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>385</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added Larissa the Priest
</commit_message>
<xml_diff>
--- a/Misc/Names and Roles.xlsx
+++ b/Misc/Names and Roles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ShiMapleLeaf\Documents\Parallel Heroes\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F86CE90-9FE7-4F47-A4DB-3F60A62DD1F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6413306-12E4-4A49-9584-CAE4B0B777CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{EF0C7BE9-5DEA-4A5F-B898-9F15494C8668}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EF0C7BE9-5DEA-4A5F-B898-9F15494C8668}"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="138">
   <si>
     <t>Clint</t>
   </si>
@@ -443,6 +443,9 @@
   </si>
   <si>
     <t>Lute</t>
+  </si>
+  <si>
+    <t>Spirits</t>
   </si>
 </sst>
 </file>
@@ -550,7 +553,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3896,7 +3899,7 @@
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -4231,11 +4234,32 @@
         <v>22</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>97</v>
+        <v>137</v>
+      </c>
+      <c r="G13" s="2">
+        <v>50</v>
+      </c>
+      <c r="H13" s="2">
+        <v>70</v>
+      </c>
+      <c r="I13" s="2">
+        <v>60</v>
+      </c>
+      <c r="J13" s="2">
+        <v>40</v>
+      </c>
+      <c r="K13" s="2">
+        <v>70</v>
+      </c>
+      <c r="L13" s="2">
+        <v>40</v>
+      </c>
+      <c r="M13" s="2">
+        <v>55</v>
       </c>
       <c r="N13" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>385</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added Inori and Marco
</commit_message>
<xml_diff>
--- a/Misc/Names and Roles.xlsx
+++ b/Misc/Names and Roles.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ShiMapleLeaf\Documents\Parallel Heroes\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6413306-12E4-4A49-9584-CAE4B0B777CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CFE6D44-D7B0-4A19-BC22-69A5DCF6BF5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EF0C7BE9-5DEA-4A5F-B898-9F15494C8668}"/>
   </bookViews>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -633,7 +635,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp30.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp31.xml><?xml version="1.0" encoding="utf-8"?>
@@ -649,7 +651,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp34.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp35.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3898,8 +3900,8 @@
   <sheetPr codeName="Blad1"/>
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -4687,9 +4689,30 @@
       <c r="D31" s="2" t="s">
         <v>134</v>
       </c>
+      <c r="G31" s="2">
+        <v>60</v>
+      </c>
+      <c r="H31" s="2">
+        <v>80</v>
+      </c>
+      <c r="I31" s="2">
+        <v>55</v>
+      </c>
+      <c r="J31" s="2">
+        <v>45</v>
+      </c>
+      <c r="K31" s="2">
+        <v>45</v>
+      </c>
+      <c r="L31" s="2">
+        <v>40</v>
+      </c>
+      <c r="M31" s="2">
+        <v>65</v>
+      </c>
       <c r="N31" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>390</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
@@ -4759,9 +4782,30 @@
       <c r="D35" s="2" t="s">
         <v>104</v>
       </c>
+      <c r="G35" s="2">
+        <v>70</v>
+      </c>
+      <c r="H35" s="2">
+        <v>50</v>
+      </c>
+      <c r="I35" s="2">
+        <v>65</v>
+      </c>
+      <c r="J35" s="2">
+        <v>50</v>
+      </c>
+      <c r="K35" s="2">
+        <v>70</v>
+      </c>
+      <c r="L35" s="2">
+        <v>40</v>
+      </c>
+      <c r="M35" s="2">
+        <v>40</v>
+      </c>
       <c r="N35" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>385</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>